<commit_message>
Updated test spreadsheet to include reference
</commit_message>
<xml_diff>
--- a/source/SuperSimple.Spreadsheets.ConsoleTest/test.xlsx
+++ b/source/SuperSimple.Spreadsheets.ConsoleTest/test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Open Source\SuperSimple.Spreadsheets\source\SuperSimple.Spreadsheets.ConsoleTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source code\Repos\SuperSimple\SuperSimple.Spreadsheets\source\SuperSimple.Spreadsheets.ConsoleTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8554B5-E61A-4BE6-A907-02491C9A8701}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="0" windowWidth="34920" windowHeight="4695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>Id</t>
   </si>
@@ -123,9 +124,6 @@
   </si>
   <si>
     <t>Advice message for Update Tracking Number</t>
-  </si>
-  <si>
-    <t>Advice message for Re-print Shipping Labels</t>
   </si>
   <si>
     <t>Success message for Cancel Collection With / Without Refund</t>
@@ -564,7 +562,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -632,31 +630,31 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
       </c>
       <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2" t="s">
         <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -670,28 +668,28 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -702,28 +700,28 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -737,25 +735,25 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -769,28 +767,28 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -801,22 +799,22 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
         <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
         <v>32</v>
@@ -830,25 +828,26 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
         <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" t="s">
-        <v>33</v>
+        <v>52</v>
+      </c>
+      <c r="K8" t="str">
+        <f>K7</f>
+        <v>Advice message for Update Tracking Number</v>
       </c>
     </row>
   </sheetData>

</xml_diff>